<commit_message>
Several changes, improvements and overall revisions
</commit_message>
<xml_diff>
--- a/public/cameras.xlsx
+++ b/public/cameras.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55119\Downloads\Grupo WKR\Node JS\newguardiao\guardiaotwo\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC66D6-0E78-449F-9428-89F3FF8CC5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AC7C87-3466-43C7-A0AD-D81FCEDC3838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD031D0F-474D-425A-BDE8-73A5437025BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BD031D0F-474D-425A-BDE8-73A5437025BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>https://nginx.megaguardiao.com.br/live/hls/m-lojagil.m3u8</t>
   </si>
   <si>
-    <t>https://nginx.megaguardiao.com.br/live/hls/m-ozeaisportao.m3u8</t>
-  </si>
-  <si>
     <t>Ozeias - Garagem</t>
   </si>
   <si>
@@ -113,18 +110,6 @@
     <t>m-ozeaisgaragem</t>
   </si>
   <si>
-    <t>http://nginx.megaguardiao.com.br/live/hls/m-mbtosa1.m3u8</t>
-  </si>
-  <si>
-    <t>http://nginx.megaguardiao.com.br/live/hls/m-mbtosa2.m3u8</t>
-  </si>
-  <si>
-    <t>http://nginx.megaguardiao.com.br/live/hls/mbtosa3.m3u8</t>
-  </si>
-  <si>
-    <t>http://nginx.megaguardiao.com.br/live/hls/lpr.m3u8</t>
-  </si>
-  <si>
     <t>m-mbtosa1</t>
   </si>
   <si>
@@ -147,6 +132,21 @@
   </si>
   <si>
     <t>Megabit LPR</t>
+  </si>
+  <si>
+    <t>https://nginx.megaguardiao.com.br/live/hls/m-mbtosa2.m3u8</t>
+  </si>
+  <si>
+    <t>https://nginx.megaguardiao.com.br/live/hls/m-mbtosa1.m3u8</t>
+  </si>
+  <si>
+    <t>https://nginx.megaguardiao.com.br/live/hls/mbtosa3.m3u8</t>
+  </si>
+  <si>
+    <t>https://nginx.megaguardiao.com.br/live/hls/lpr.m3u8</t>
+  </si>
+  <si>
+    <t>https://streaming.megaguardiao.com.br/click190-cloud/3e026423e27946aba02e.stream/chunklist_w1960725029.m3u8</t>
   </si>
 </sst>
 </file>
@@ -538,15 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976B245D-9BA0-418A-BA3A-295B78700C18}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="10" max="10" width="12.109375" customWidth="1"/>
     <col min="11" max="11" width="82.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -591,7 +592,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -618,7 +619,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -626,7 +627,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -658,10 +659,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -688,15 +689,15 @@
         <v>13</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -723,15 +724,15 @@
         <v>13</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -758,15 +759,15 @@
         <v>13</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -793,15 +794,15 @@
         <v>12</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -828,20 +829,22 @@
         <v>12</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{D3EAC757-91FA-4D9A-BAB2-BB58B2AFABD6}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{CC6B3970-9B7A-440F-85E1-1A01ED9EB9F6}"/>
-    <hyperlink ref="K4" r:id="rId3" xr:uid="{5216453A-6E4F-4D0F-BEF4-2DF51B2260DD}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{DD4F2BFF-6812-407C-9F19-DB9C744CEC3F}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{BE7AD7D9-0492-400E-B9D7-9A799D4E07EB}"/>
-    <hyperlink ref="K7" r:id="rId6" xr:uid="{E5E28134-C414-484E-B6C1-A7DAA8825F34}"/>
-    <hyperlink ref="K8" r:id="rId7" xr:uid="{A71E7BEC-F47A-45D1-8CCB-FD91351BF4BC}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{CC6B3970-9B7A-440F-85E1-1A01ED9EB9F6}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{5216453A-6E4F-4D0F-BEF4-2DF51B2260DD}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{DD4F2BFF-6812-407C-9F19-DB9C744CEC3F}"/>
+    <hyperlink ref="K6" r:id="rId4" xr:uid="{BE7AD7D9-0492-400E-B9D7-9A799D4E07EB}"/>
+    <hyperlink ref="K7" r:id="rId5" xr:uid="{E5E28134-C414-484E-B6C1-A7DAA8825F34}"/>
+    <hyperlink ref="K8" r:id="rId6" xr:uid="{A71E7BEC-F47A-45D1-8CCB-FD91351BF4BC}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>